<commit_message>
ci platform mvc files updated
</commit_message>
<xml_diff>
--- a/CI Project/CI-DB/CI PLATEFORM SCHEEMA.xlsx
+++ b/CI Project/CI-DB/CI PLATEFORM SCHEEMA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\Tatva Projects\CI Project\CI-DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506B824A-F1AA-4992-B813-02976DF99346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB319BF-BAC4-4332-9236-EA41A4DC9FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{310437BF-ADAC-461E-A405-DE8A102E9B49}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="111">
   <si>
     <t>CI Plateform Databse</t>
   </si>
@@ -467,27 +466,27 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -806,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996707CD-DEEA-4255-A655-89B263436B90}">
   <dimension ref="A1:R162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129:I129"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="97" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,68 +820,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
     </row>
     <row r="4" spans="1:18" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1152,46 +1151,46 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1465,46 +1464,46 @@
       </c>
     </row>
     <row r="54" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G56" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H56" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1571,46 +1570,46 @@
       </c>
     </row>
     <row r="64" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G66" s="3" t="s">
+      <c r="G66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="3" t="s">
+      <c r="H66" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1657,46 +1656,46 @@
       </c>
     </row>
     <row r="73" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D75" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E75" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="F75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="G75" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H75" s="3" t="s">
+      <c r="H75" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1743,46 +1742,46 @@
       </c>
     </row>
     <row r="82" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
-      <c r="L82" s="2"/>
-      <c r="M82" s="2"/>
-      <c r="N82" s="2"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D84" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E84" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F84" s="3" t="s">
+      <c r="F84" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G84" s="3" t="s">
+      <c r="G84" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="H84" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1840,41 +1839,41 @@
       </c>
     </row>
     <row r="92" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B92" s="6"/>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="6"/>
-      <c r="F92" s="6"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6"/>
-      <c r="I92" s="6"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C94" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E94" s="5" t="s">
+      <c r="E94" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F94" s="5" t="s">
+      <c r="F94" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G94" s="5" t="s">
+      <c r="G94" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H94" s="5" t="s">
+      <c r="H94" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1919,41 +1918,41 @@
       </c>
     </row>
     <row r="101" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A101" s="6" t="s">
+      <c r="A101" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="C103" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E103" s="5" t="s">
+      <c r="E103" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F103" s="5" t="s">
+      <c r="F103" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G103" s="5" t="s">
+      <c r="G103" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H103" s="5" t="s">
+      <c r="H103" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1998,41 +1997,41 @@
       </c>
     </row>
     <row r="109" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A109" s="6" t="s">
+      <c r="A109" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B109" s="6"/>
-      <c r="C109" s="6"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="6"/>
-      <c r="F109" s="6"/>
-      <c r="G109" s="6"/>
-      <c r="H109" s="6"/>
-      <c r="I109" s="6"/>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="3"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="5" t="s">
+      <c r="A111" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B111" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C111" s="5" t="s">
+      <c r="C111" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="D111" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E111" s="5" t="s">
+      <c r="E111" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F111" s="5" t="s">
+      <c r="F111" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G111" s="5" t="s">
+      <c r="G111" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H111" s="5" t="s">
+      <c r="H111" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2077,41 +2076,41 @@
       </c>
     </row>
     <row r="117" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A117" s="6" t="s">
+      <c r="A117" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B117" s="6"/>
-      <c r="C117" s="6"/>
-      <c r="D117" s="6"/>
-      <c r="E117" s="6"/>
-      <c r="F117" s="6"/>
-      <c r="G117" s="6"/>
-      <c r="H117" s="6"/>
-      <c r="I117" s="6"/>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="3"/>
+      <c r="I117" s="3"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B119" s="5" t="s">
+      <c r="B119" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C119" s="5" t="s">
+      <c r="C119" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D119" s="5" t="s">
+      <c r="D119" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E119" s="5" t="s">
+      <c r="E119" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F119" s="5" t="s">
+      <c r="F119" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G119" s="5" t="s">
+      <c r="G119" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H119" s="5" t="s">
+      <c r="H119" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2220,41 +2219,41 @@
       </c>
     </row>
     <row r="129" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A129" s="6" t="s">
+      <c r="A129" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B129" s="6"/>
-      <c r="C129" s="6"/>
-      <c r="D129" s="6"/>
-      <c r="E129" s="6"/>
-      <c r="F129" s="6"/>
-      <c r="G129" s="6"/>
-      <c r="H129" s="6"/>
-      <c r="I129" s="6"/>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="3"/>
+      <c r="I129" s="3"/>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A131" s="5" t="s">
+      <c r="A131" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B131" s="5" t="s">
+      <c r="B131" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C131" s="5" t="s">
+      <c r="C131" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D131" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E131" s="5" t="s">
+      <c r="E131" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F131" s="5" t="s">
+      <c r="F131" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G131" s="5" t="s">
+      <c r="G131" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H131" s="5" t="s">
+      <c r="H131" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2333,58 +2332,58 @@
       </c>
     </row>
     <row r="139" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A139" s="8" t="s">
+      <c r="A139" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B139" s="9"/>
-      <c r="C139" s="9"/>
-      <c r="D139" s="9"/>
-      <c r="E139" s="9"/>
-      <c r="F139" s="9"/>
-      <c r="G139" s="9"/>
-      <c r="H139" s="9"/>
-      <c r="I139" s="9"/>
-      <c r="J139" s="9"/>
-      <c r="K139" s="9"/>
-      <c r="L139" s="9"/>
-      <c r="M139" s="9"/>
+      <c r="B139" s="7"/>
+      <c r="C139" s="7"/>
+      <c r="D139" s="7"/>
+      <c r="E139" s="7"/>
+      <c r="F139" s="7"/>
+      <c r="G139" s="7"/>
+      <c r="H139" s="7"/>
+      <c r="I139" s="7"/>
+      <c r="J139" s="7"/>
+      <c r="K139" s="7"/>
+      <c r="L139" s="7"/>
+      <c r="M139" s="7"/>
     </row>
     <row r="141" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
-      <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
-      <c r="I141" s="2"/>
+      <c r="B141" s="4"/>
+      <c r="C141" s="4"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
+      <c r="H141" s="4"/>
+      <c r="I141" s="4"/>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A143" s="5" t="s">
+      <c r="A143" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B143" s="5" t="s">
+      <c r="B143" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C143" s="5" t="s">
+      <c r="C143" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D143" s="5" t="s">
+      <c r="D143" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E143" s="5" t="s">
+      <c r="E143" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F143" s="5" t="s">
+      <c r="F143" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G143" s="5" t="s">
+      <c r="G143" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H143" s="5" t="s">
+      <c r="H143" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2401,6 +2400,9 @@
       <c r="E145" t="s">
         <v>22</v>
       </c>
+      <c r="F145" t="s">
+        <v>41</v>
+      </c>
       <c r="G145" t="s">
         <v>16</v>
       </c>
@@ -2496,41 +2498,41 @@
       </c>
     </row>
     <row r="154" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A154" s="6" t="s">
+      <c r="A154" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="2"/>
-      <c r="F154" s="2"/>
-      <c r="G154" s="2"/>
-      <c r="H154" s="2"/>
-      <c r="I154" s="2"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="4"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
+      <c r="H154" s="4"/>
+      <c r="I154" s="4"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A156" s="5" t="s">
+      <c r="A156" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B156" s="5" t="s">
+      <c r="B156" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C156" s="5" t="s">
+      <c r="C156" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D156" s="5" t="s">
+      <c r="D156" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E156" s="5" t="s">
+      <c r="E156" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F156" s="5" t="s">
+      <c r="F156" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G156" s="5" t="s">
+      <c r="G156" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H156" s="5" t="s">
+      <c r="H156" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2624,6 +2626,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="A26:N26"/>
+    <mergeCell ref="A92:I92"/>
+    <mergeCell ref="A101:I101"/>
     <mergeCell ref="A154:I154"/>
     <mergeCell ref="A109:I109"/>
     <mergeCell ref="A117:I117"/>
@@ -2634,11 +2641,6 @@
     <mergeCell ref="A82:N82"/>
     <mergeCell ref="A139:M139"/>
     <mergeCell ref="A141:I141"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A4:N4"/>
-    <mergeCell ref="A26:N26"/>
-    <mergeCell ref="A92:I92"/>
-    <mergeCell ref="A101:I101"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>